<commit_message>
Crime Dashboard Draft 1
</commit_message>
<xml_diff>
--- a/Crimes against Women/filtered data/Data By Year (CAW).xlsx
+++ b/Crimes against Women/filtered data/Data By Year (CAW).xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhanu\Desktop\Data Analytics\Projects\Crime Dashboard\Crimes against Women\filtered data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14662762-CB2F-43ED-8ECB-4ABB595D5828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A366FCC-CCD7-49E9-B311-F2AD91DF5A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4668" yWindow="2328" windowWidth="17280" windowHeight="10188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5088" yWindow="564" windowWidth="17280" windowHeight="10188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -467,35 +476,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W33" workbookViewId="0">
-      <selection activeCell="Z48" sqref="Z48"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="46.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="48.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="67.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="69.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="47.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="60" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="73" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="74.88671875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="71.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="62.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.77734375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="63.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="72.44140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="45" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="46.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
@@ -625,7 +635,7 @@
         <v>25</v>
       </c>
       <c r="Q2">
-        <v>208</v>
+        <v>1</v>
       </c>
       <c r="R2">
         <v>233</v>
@@ -1193,7 +1203,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
@@ -1270,7 +1280,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -1347,7 +1357,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
@@ -1424,7 +1434,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
@@ -1501,7 +1511,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
@@ -1578,7 +1588,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
@@ -1655,7 +1665,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
@@ -1732,7 +1742,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
@@ -1809,7 +1819,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
@@ -1886,7 +1896,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -1963,7 +1973,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
@@ -2040,7 +2050,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>27</v>
@@ -2117,7 +2127,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>28</v>
@@ -2194,7 +2204,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
@@ -2271,7 +2281,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>30</v>
@@ -2348,7 +2358,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>31</v>
@@ -2425,7 +2435,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
@@ -2502,7 +2512,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>33</v>
@@ -2579,7 +2589,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>34</v>
@@ -2656,7 +2666,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
@@ -2733,7 +2743,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>36</v>
@@ -2887,7 +2897,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>38</v>
@@ -2964,7 +2974,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>39</v>
@@ -3041,7 +3051,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>24</v>
@@ -3118,7 +3128,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
@@ -3195,7 +3205,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>26</v>
@@ -3272,7 +3282,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>27</v>
@@ -3349,7 +3359,7 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>28</v>
@@ -3426,7 +3436,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>29</v>
@@ -3503,7 +3513,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>30</v>
@@ -3580,7 +3590,7 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>31</v>
@@ -3657,7 +3667,7 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>32</v>
@@ -3734,7 +3744,7 @@
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>33</v>
@@ -3811,7 +3821,7 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>34</v>
@@ -3888,7 +3898,7 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>35</v>
@@ -3965,7 +3975,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>36</v>
@@ -4042,7 +4052,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>37</v>
@@ -4119,7 +4129,7 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>38</v>
@@ -4196,7 +4206,7 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>39</v>

</xml_diff>